<commit_message>
se agrega pantalla de calibracion
</commit_message>
<xml_diff>
--- a/Pinout STM32.xlsx
+++ b/Pinout STM32.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RepositoriosGit\EstacionCalorPro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A543DF65-3670-4701-8FA1-17A8A42D6E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5CDB2F-EE46-4426-82ED-88E31B595D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F50C8D62-0681-441D-8638-5078836FED94}"/>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15840" xr2:uid="{F50C8D62-0681-441D-8638-5078836FED94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="82">
   <si>
     <t>Pin</t>
   </si>
@@ -279,6 +279,9 @@
   </si>
   <si>
     <t>GPIO_EXTI14</t>
+  </si>
+  <si>
+    <t>sensor teperatura analogico</t>
   </si>
 </sst>
 </file>
@@ -353,7 +356,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -402,6 +405,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -410,16 +424,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -436,7 +441,21 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -449,12 +468,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,7 +497,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>663382</xdr:colOff>
+      <xdr:colOff>166425</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
@@ -544,7 +558,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>1220027</xdr:colOff>
+      <xdr:colOff>723070</xdr:colOff>
       <xdr:row>99</xdr:row>
       <xdr:rowOff>94094</xdr:rowOff>
     </xdr:to>
@@ -918,15 +932,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F56990-E0A1-4F63-BA9D-D997C6F01975}">
   <dimension ref="I2:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="9.140625" customWidth="1"/>
     <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
@@ -939,197 +953,197 @@
   <sheetData>
     <row r="2" spans="9:20" x14ac:dyDescent="0.25">
       <c r="J2" s="2"/>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
       <c r="S2" s="2"/>
     </row>
     <row r="3" spans="9:20" x14ac:dyDescent="0.25">
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="5" t="s">
+      <c r="L3" s="1"/>
+      <c r="M3" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="4"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="3"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
     </row>
     <row r="4" spans="9:20" x14ac:dyDescent="0.25">
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="17"/>
+      <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="3" t="s">
+      <c r="N4" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="O4" s="3"/>
+      <c r="O4" s="20"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
     </row>
     <row r="5" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J5" s="20" t="s">
+      <c r="J5" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="K5" s="21"/>
-      <c r="L5" s="18" t="s">
+      <c r="K5" s="26"/>
+      <c r="L5" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="M5" s="19"/>
-      <c r="N5" s="9" t="s">
+      <c r="M5" s="24"/>
+      <c r="N5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="O5" s="9" t="s">
+      <c r="O5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="P5" s="18" t="s">
+      <c r="P5" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="20" t="s">
+      <c r="Q5" s="24"/>
+      <c r="R5" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="S5" s="21"/>
+      <c r="S5" s="26"/>
     </row>
     <row r="6" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J6" s="7"/>
-      <c r="K6" s="7" t="s">
+      <c r="J6" s="4"/>
+      <c r="K6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8" t="s">
+      <c r="L6" s="5"/>
+      <c r="M6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="9">
+      <c r="N6" s="6">
         <v>1</v>
       </c>
-      <c r="O6" s="9">
+      <c r="O6" s="6">
         <v>1</v>
       </c>
-      <c r="P6" s="8" t="s">
+      <c r="P6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="7" t="s">
+      <c r="Q6" s="5"/>
+      <c r="R6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="S6" s="7"/>
+      <c r="S6" s="4"/>
     </row>
     <row r="7" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I7" s="27" t="s">
+      <c r="I7" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="J7" s="23" t="s">
+      <c r="J7" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="K7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="8"/>
-      <c r="M7" s="11" t="s">
+      <c r="L7" s="5"/>
+      <c r="M7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="N7" s="12">
+      <c r="N7" s="9">
         <v>2</v>
       </c>
-      <c r="O7" s="12">
+      <c r="O7" s="9">
         <v>2</v>
       </c>
-      <c r="P7" s="8" t="s">
+      <c r="P7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="Q7" s="8"/>
-      <c r="R7" s="7" t="s">
+      <c r="Q7" s="5"/>
+      <c r="R7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="S7" s="7"/>
+      <c r="S7" s="4"/>
     </row>
     <row r="8" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J8" s="7"/>
-      <c r="K8" s="10" t="s">
+      <c r="J8" s="4"/>
+      <c r="K8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="8"/>
-      <c r="M8" s="11" t="s">
+      <c r="L8" s="5"/>
+      <c r="M8" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="N8" s="12">
+      <c r="N8" s="9">
         <v>3</v>
       </c>
-      <c r="O8" s="12">
+      <c r="O8" s="9">
         <v>3</v>
       </c>
-      <c r="P8" s="8" t="s">
+      <c r="P8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="7" t="s">
+      <c r="Q8" s="5"/>
+      <c r="R8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="S8" s="7"/>
+      <c r="S8" s="4"/>
     </row>
     <row r="9" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J9" s="7"/>
-      <c r="K9" s="10" t="s">
+      <c r="J9" s="4"/>
+      <c r="K9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="L9" s="8"/>
-      <c r="M9" s="11" t="s">
+      <c r="L9" s="5"/>
+      <c r="M9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="N9" s="12">
+      <c r="N9" s="9">
         <v>4</v>
       </c>
-      <c r="O9" s="12">
+      <c r="O9" s="9">
         <v>4</v>
       </c>
-      <c r="P9" s="13" t="s">
+      <c r="P9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="14" t="s">
+      <c r="Q9" s="10"/>
+      <c r="R9" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J10" s="7"/>
-      <c r="K10" s="7" t="s">
+      <c r="J10" s="4"/>
+      <c r="K10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="L10" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="M10" s="15" t="s">
+      <c r="M10" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="N10" s="12">
+      <c r="N10" s="9">
         <v>5</v>
       </c>
-      <c r="O10" s="12">
+      <c r="O10" s="9">
         <v>5</v>
       </c>
-      <c r="P10" s="13" t="s">
+      <c r="P10" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="Q10" s="13" t="s">
+      <c r="Q10" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="R10" s="14" t="s">
+      <c r="R10" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="S10" s="22" t="s">
+      <c r="S10" s="14" t="s">
         <v>58</v>
       </c>
       <c r="T10" t="s">
@@ -1137,194 +1151,197 @@
       </c>
     </row>
     <row r="11" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J11" s="23" t="s">
+      <c r="J11" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="K11" s="16" t="s">
+      <c r="K11" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="L11" s="15" t="s">
+      <c r="L11" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="M11" s="15" t="s">
+      <c r="M11" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="N11" s="12">
+      <c r="N11" s="9">
         <v>6</v>
       </c>
-      <c r="O11" s="12">
+      <c r="O11" s="9">
         <v>6</v>
       </c>
-      <c r="P11" s="13" t="s">
+      <c r="P11" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="Q11" s="13" t="s">
+      <c r="Q11" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="R11" s="14" t="s">
+      <c r="R11" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="S11" s="22" t="s">
+      <c r="S11" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="12" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J12" s="23" t="s">
+      <c r="J12" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="K12" s="16" t="s">
+      <c r="K12" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="L12" s="15" t="s">
+      <c r="L12" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="15" t="s">
+      <c r="M12" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="N12" s="12">
+      <c r="N12" s="9">
         <v>7</v>
       </c>
-      <c r="O12" s="12">
+      <c r="O12" s="9">
         <v>7</v>
       </c>
-      <c r="P12" s="13" t="s">
+      <c r="P12" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="Q12" s="13" t="s">
+      <c r="Q12" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="R12" s="14" t="s">
+      <c r="R12" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="S12" s="22" t="s">
+      <c r="S12" s="14" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="13" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J13" s="23" t="s">
+      <c r="J13" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="K13" s="16" t="s">
+      <c r="K13" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="L13" s="15" t="s">
+      <c r="L13" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="M13" s="15" t="s">
+      <c r="M13" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="N13" s="12">
+      <c r="N13" s="9">
         <v>8</v>
       </c>
-      <c r="O13" s="12">
+      <c r="O13" s="9">
         <v>8</v>
       </c>
-      <c r="P13" s="13" t="s">
+      <c r="P13" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="Q13" s="13" t="s">
+      <c r="Q13" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="R13" s="14" t="s">
+      <c r="R13" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="S13" s="22" t="s">
+      <c r="S13" s="14" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="14" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J14" s="23" t="s">
+      <c r="J14" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="K14" s="16" t="s">
+      <c r="K14" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="L14" s="15" t="s">
+      <c r="L14" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="M14" s="15" t="s">
+      <c r="M14" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="N14" s="12">
+      <c r="N14" s="9">
         <v>9</v>
       </c>
-      <c r="O14" s="12">
+      <c r="O14" s="9">
         <v>9</v>
       </c>
-      <c r="P14" s="13" t="s">
+      <c r="P14" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="Q14" s="13" t="s">
+      <c r="Q14" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="R14" s="26" t="s">
+      <c r="R14" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="S14" s="22" t="s">
+      <c r="S14" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="T14" s="27" t="s">
+      <c r="T14" s="19" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="15" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="K15" s="25" t="s">
+      <c r="J15" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="K15" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="L15" s="15" t="s">
+      <c r="L15" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="M15" s="15" t="s">
+      <c r="M15" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="N15" s="12">
+      <c r="N15" s="9">
         <v>10</v>
       </c>
-      <c r="O15" s="12">
+      <c r="O15" s="9">
         <v>10</v>
       </c>
-      <c r="P15" s="13" t="s">
+      <c r="P15" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="Q15" s="13" t="s">
+      <c r="Q15" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="R15" s="14" t="s">
+      <c r="R15" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="S15" s="22" t="s">
+      <c r="S15" s="14" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="16" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J16" s="23" t="s">
+      <c r="J16" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="K16" s="16" t="s">
+      <c r="K16" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="L16" s="15" t="s">
+      <c r="L16" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="M16" s="15" t="s">
+      <c r="M16" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="N16" s="12">
+      <c r="N16" s="9">
         <v>11</v>
       </c>
-      <c r="O16" s="12">
+      <c r="O16" s="9">
         <v>11</v>
       </c>
-      <c r="P16" s="15" t="s">
+      <c r="P16" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="Q16" s="15" t="s">
+      <c r="Q16" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="R16" s="16" t="s">
+      <c r="R16" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="S16" s="23" t="s">
+      <c r="S16" s="15" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1332,186 +1349,186 @@
       <c r="I17" t="s">
         <v>75</v>
       </c>
-      <c r="J17" s="23" t="s">
+      <c r="J17" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="K17" s="16" t="s">
+      <c r="K17" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="L17" s="15" t="s">
+      <c r="L17" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="M17" s="15" t="s">
+      <c r="M17" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="N17" s="12">
+      <c r="N17" s="9">
         <v>12</v>
       </c>
-      <c r="O17" s="12">
+      <c r="O17" s="9">
         <v>12</v>
       </c>
-      <c r="P17" s="15" t="s">
+      <c r="P17" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="16" t="s">
+      <c r="Q17" s="12"/>
+      <c r="R17" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="S17" s="16"/>
+      <c r="S17" s="13"/>
     </row>
     <row r="18" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J18" s="23" t="s">
+      <c r="J18" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="K18" s="16" t="s">
+      <c r="K18" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="L18" s="13" t="s">
+      <c r="L18" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="M18" s="13" t="s">
+      <c r="M18" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="N18" s="12">
+      <c r="N18" s="9">
         <v>13</v>
       </c>
-      <c r="O18" s="12">
+      <c r="O18" s="9">
         <v>13</v>
       </c>
-      <c r="P18" s="15" t="s">
+      <c r="P18" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="16" t="s">
+      <c r="Q18" s="12"/>
+      <c r="R18" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="S18" s="16"/>
+      <c r="S18" s="13"/>
     </row>
     <row r="19" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J19" s="23" t="s">
+      <c r="J19" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="K19" s="14" t="s">
+      <c r="K19" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="L19" s="13" t="s">
+      <c r="L19" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="M19" s="13" t="s">
+      <c r="M19" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="N19" s="12">
+      <c r="N19" s="9">
         <v>14</v>
       </c>
-      <c r="O19" s="12">
+      <c r="O19" s="9">
         <v>14</v>
       </c>
-      <c r="P19" s="15" t="s">
+      <c r="P19" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="Q19" s="15" t="s">
+      <c r="Q19" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="R19" s="16" t="s">
+      <c r="R19" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="S19" s="23" t="s">
+      <c r="S19" s="15" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="20" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J20" s="22" t="s">
+      <c r="J20" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="K20" s="14" t="s">
+      <c r="K20" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="L20" s="13" t="s">
+      <c r="L20" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="M20" s="13" t="s">
+      <c r="M20" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="N20" s="12">
+      <c r="N20" s="9">
         <v>15</v>
       </c>
-      <c r="O20" s="12">
+      <c r="O20" s="9">
         <v>15</v>
       </c>
-      <c r="P20" s="15" t="s">
+      <c r="P20" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="Q20" s="15" t="s">
+      <c r="Q20" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="R20" s="16" t="s">
+      <c r="R20" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="S20" s="23" t="s">
+      <c r="S20" s="15" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="21" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I21" s="27" t="s">
+      <c r="I21" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="J21" s="24" t="s">
+      <c r="J21" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="K21" s="10" t="s">
+      <c r="K21" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="L21" s="11" t="s">
+      <c r="L21" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="M21" s="11" t="s">
+      <c r="M21" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="N21" s="12">
+      <c r="N21" s="9">
         <v>16</v>
       </c>
-      <c r="O21" s="12">
+      <c r="O21" s="9">
         <v>16</v>
       </c>
-      <c r="P21" s="15" t="s">
+      <c r="P21" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="16" t="s">
+      <c r="Q21" s="12"/>
+      <c r="R21" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="S21" s="16"/>
+      <c r="S21" s="13"/>
     </row>
     <row r="22" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I22" s="27" t="s">
+      <c r="I22" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="J22" s="22" t="s">
+      <c r="J22" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="K22" s="14" t="s">
+      <c r="K22" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8" t="s">
+      <c r="L22" s="5"/>
+      <c r="M22" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="N22" s="12">
+      <c r="N22" s="9">
         <v>17</v>
       </c>
-      <c r="O22" s="12">
+      <c r="O22" s="9">
         <v>17</v>
       </c>
-      <c r="P22" s="13" t="s">
+      <c r="P22" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="Q22" s="13" t="s">
+      <c r="Q22" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="R22" s="14" t="s">
+      <c r="R22" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="S22" s="22" t="s">
+      <c r="S22" s="14" t="s">
         <v>55</v>
       </c>
       <c r="T22" t="s">
@@ -1519,78 +1536,78 @@
       </c>
     </row>
     <row r="23" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J23" s="7"/>
-      <c r="K23" s="7" t="s">
+      <c r="J23" s="4"/>
+      <c r="K23" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8" t="s">
+      <c r="L23" s="5"/>
+      <c r="M23" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="N23" s="12">
+      <c r="N23" s="9">
         <v>18</v>
       </c>
-      <c r="O23" s="12">
+      <c r="O23" s="9">
         <v>18</v>
       </c>
-      <c r="P23" s="13" t="s">
+      <c r="P23" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="14" t="s">
+      <c r="Q23" s="10"/>
+      <c r="R23" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="S23" s="14"/>
+      <c r="S23" s="11"/>
     </row>
     <row r="24" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J24" s="7"/>
-      <c r="K24" s="7" t="s">
+      <c r="J24" s="4"/>
+      <c r="K24" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8" t="s">
+      <c r="L24" s="5"/>
+      <c r="M24" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="N24" s="12">
+      <c r="N24" s="9">
         <v>19</v>
       </c>
-      <c r="O24" s="12">
+      <c r="O24" s="9">
         <v>19</v>
       </c>
-      <c r="P24" s="13" t="s">
+      <c r="P24" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q24" s="13"/>
-      <c r="R24" s="14" t="s">
+      <c r="Q24" s="10"/>
+      <c r="R24" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="S24" s="14"/>
+      <c r="S24" s="11"/>
     </row>
     <row r="25" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J25" s="7"/>
-      <c r="K25" s="7" t="s">
+      <c r="J25" s="4"/>
+      <c r="K25" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8" t="s">
+      <c r="L25" s="5"/>
+      <c r="M25" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="N25" s="12">
+      <c r="N25" s="9">
         <v>20</v>
       </c>
-      <c r="O25" s="12">
+      <c r="O25" s="9">
         <v>20</v>
       </c>
-      <c r="P25" s="13" t="s">
+      <c r="P25" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="Q25" s="13" t="s">
+      <c r="Q25" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="R25" s="14" t="s">
+      <c r="R25" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="S25" s="22" t="s">
+      <c r="S25" s="14" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se agrega configuracion de rampas detemperatura
</commit_message>
<xml_diff>
--- a/Pinout STM32.xlsx
+++ b/Pinout STM32.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RepositoriosGit\EstacionCalorPro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDDBF70-0D40-42C7-BF6B-9D3637230B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D622EC5F-4657-4FE8-A6BA-6D6D1DF6F009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F50C8D62-0681-441D-8638-5078836FED94}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="84">
   <si>
     <t>Pin</t>
   </si>
@@ -278,17 +278,23 @@
     <t>GPIO_EXTI15</t>
   </si>
   <si>
-    <t>GPIO_EXTI14</t>
-  </si>
-  <si>
     <t>sensor teperatura analogico</t>
+  </si>
+  <si>
+    <t>Boton2</t>
+  </si>
+  <si>
+    <t>GPIO_EXTI13</t>
+  </si>
+  <si>
+    <t>A4 (ADC1_IN4)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,8 +330,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -359,6 +371,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -427,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -446,11 +476,10 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -460,19 +489,25 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -936,7 +971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F56990-E0A1-4F63-BA9D-D997C6F01975}">
   <dimension ref="I2:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
@@ -957,28 +992,28 @@
   <sheetData>
     <row r="2" spans="9:20" x14ac:dyDescent="0.25">
       <c r="J2" s="2"/>
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
       <c r="S2" s="2"/>
     </row>
     <row r="3" spans="9:20" x14ac:dyDescent="0.25">
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="18" t="s">
+      <c r="M3" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="N3" s="18"/>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
@@ -988,46 +1023,46 @@
       <c r="K4" s="2"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="17" t="s">
+      <c r="N4" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="O4" s="17"/>
+      <c r="O4" s="16"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
     </row>
     <row r="5" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J5" s="20" t="s">
+      <c r="J5" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="K5" s="21"/>
-      <c r="L5" s="22" t="s">
+      <c r="K5" s="22"/>
+      <c r="L5" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="M5" s="23"/>
+      <c r="M5" s="20"/>
       <c r="N5" s="5" t="s">
         <v>0</v>
       </c>
       <c r="O5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="P5" s="22" t="s">
+      <c r="P5" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="20" t="s">
+      <c r="Q5" s="20"/>
+      <c r="R5" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="S5" s="21"/>
+      <c r="S5" s="22"/>
     </row>
     <row r="6" spans="9:20" x14ac:dyDescent="0.25">
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24" t="s">
+      <c r="L6" s="15"/>
+      <c r="M6" s="15" t="s">
         <v>21</v>
       </c>
       <c r="N6" s="5">
@@ -1036,27 +1071,27 @@
       <c r="O6" s="5">
         <v>1</v>
       </c>
-      <c r="P6" s="24" t="s">
+      <c r="P6" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="Q6" s="24"/>
+      <c r="Q6" s="15"/>
       <c r="R6" s="4" t="s">
         <v>1</v>
       </c>
       <c r="S6" s="4"/>
     </row>
     <row r="7" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I7" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="J7" s="11" t="s">
+      <c r="I7" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="J7" s="24" t="s">
         <v>52</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24" t="s">
+      <c r="L7" s="15"/>
+      <c r="M7" s="15" t="s">
         <v>22</v>
       </c>
       <c r="N7" s="7">
@@ -1065,10 +1100,10 @@
       <c r="O7" s="7">
         <v>2</v>
       </c>
-      <c r="P7" s="24" t="s">
+      <c r="P7" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Q7" s="24"/>
+      <c r="Q7" s="15"/>
       <c r="R7" s="4" t="s">
         <v>2</v>
       </c>
@@ -1079,8 +1114,8 @@
       <c r="K8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24" t="s">
+      <c r="L8" s="15"/>
+      <c r="M8" s="15" t="s">
         <v>23</v>
       </c>
       <c r="N8" s="7">
@@ -1089,10 +1124,10 @@
       <c r="O8" s="7">
         <v>3</v>
       </c>
-      <c r="P8" s="24" t="s">
+      <c r="P8" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="Q8" s="24"/>
+      <c r="Q8" s="15"/>
       <c r="R8" s="4" t="s">
         <v>3</v>
       </c>
@@ -1103,8 +1138,8 @@
       <c r="K9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24" t="s">
+      <c r="L9" s="15"/>
+      <c r="M9" s="15" t="s">
         <v>24</v>
       </c>
       <c r="N9" s="7">
@@ -1113,10 +1148,10 @@
       <c r="O9" s="7">
         <v>4</v>
       </c>
-      <c r="P9" s="24" t="s">
+      <c r="P9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="Q9" s="24"/>
+      <c r="Q9" s="15"/>
       <c r="R9" s="8" t="s">
         <v>4</v>
       </c>
@@ -1126,10 +1161,10 @@
       <c r="K10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="L10" s="24" t="s">
+      <c r="L10" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="M10" s="24" t="s">
+      <c r="M10" s="15" t="s">
         <v>25</v>
       </c>
       <c r="N10" s="7">
@@ -1138,16 +1173,16 @@
       <c r="O10" s="7">
         <v>5</v>
       </c>
-      <c r="P10" s="24" t="s">
+      <c r="P10" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="Q10" s="24" t="s">
+      <c r="Q10" s="15" t="s">
         <v>58</v>
       </c>
       <c r="R10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="S10" s="10" t="s">
+      <c r="S10" s="26" t="s">
         <v>58</v>
       </c>
       <c r="T10" t="s">
@@ -1159,10 +1194,10 @@
       <c r="K11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="L11" s="24" t="s">
+      <c r="L11" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="M11" s="24" t="s">
+      <c r="M11" s="15" t="s">
         <v>26</v>
       </c>
       <c r="N11" s="7">
@@ -1171,10 +1206,10 @@
       <c r="O11" s="7">
         <v>6</v>
       </c>
-      <c r="P11" s="24" t="s">
+      <c r="P11" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="Q11" s="24" t="s">
+      <c r="Q11" s="15" t="s">
         <v>46</v>
       </c>
       <c r="R11" s="8" t="s">
@@ -1189,10 +1224,10 @@
       <c r="K12" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="L12" s="24" t="s">
+      <c r="L12" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="24" t="s">
+      <c r="M12" s="15" t="s">
         <v>27</v>
       </c>
       <c r="N12" s="7">
@@ -1201,10 +1236,10 @@
       <c r="O12" s="7">
         <v>7</v>
       </c>
-      <c r="P12" s="24" t="s">
+      <c r="P12" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="Q12" s="24" t="s">
+      <c r="Q12" s="15" t="s">
         <v>45</v>
       </c>
       <c r="R12" s="8" t="s">
@@ -1219,10 +1254,10 @@
       <c r="K13" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="L13" s="24" t="s">
+      <c r="L13" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="M13" s="24" t="s">
+      <c r="M13" s="15" t="s">
         <v>28</v>
       </c>
       <c r="N13" s="7">
@@ -1231,10 +1266,10 @@
       <c r="O13" s="7">
         <v>8</v>
       </c>
-      <c r="P13" s="24" t="s">
+      <c r="P13" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="Q13" s="24" t="s">
+      <c r="Q13" s="15" t="s">
         <v>49</v>
       </c>
       <c r="R13" s="8" t="s">
@@ -1251,10 +1286,10 @@
       <c r="K14" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="L14" s="24" t="s">
+      <c r="L14" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="M14" s="24" t="s">
+      <c r="M14" s="15" t="s">
         <v>29</v>
       </c>
       <c r="N14" s="7">
@@ -1263,33 +1298,33 @@
       <c r="O14" s="7">
         <v>9</v>
       </c>
-      <c r="P14" s="24" t="s">
+      <c r="P14" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="Q14" s="24" t="s">
+      <c r="Q14" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="R14" s="14" t="s">
+      <c r="R14" s="12" t="s">
         <v>9</v>
       </c>
       <c r="S14" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="T14" s="15" t="s">
+      <c r="T14" s="13" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="15" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J15" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="K15" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="L15" s="24" t="s">
+      <c r="J15" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="L15" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="M15" s="24" t="s">
+      <c r="M15" s="15" t="s">
         <v>30</v>
       </c>
       <c r="N15" s="7">
@@ -1298,10 +1333,10 @@
       <c r="O15" s="7">
         <v>10</v>
       </c>
-      <c r="P15" s="24" t="s">
+      <c r="P15" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="Q15" s="24" t="s">
+      <c r="Q15" s="15" t="s">
         <v>51</v>
       </c>
       <c r="R15" s="8" t="s">
@@ -1312,16 +1347,16 @@
       </c>
     </row>
     <row r="16" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J16" s="11" t="s">
+      <c r="J16" s="28" t="s">
         <v>60</v>
       </c>
       <c r="K16" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="L16" s="24" t="s">
+      <c r="L16" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="M16" s="24" t="s">
+      <c r="M16" s="15" t="s">
         <v>31</v>
       </c>
       <c r="N16" s="7">
@@ -1330,10 +1365,10 @@
       <c r="O16" s="7">
         <v>11</v>
       </c>
-      <c r="P16" s="24" t="s">
+      <c r="P16" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="Q16" s="24" t="s">
+      <c r="Q16" s="15" t="s">
         <v>50</v>
       </c>
       <c r="R16" s="9" t="s">
@@ -1347,16 +1382,16 @@
       <c r="I17" t="s">
         <v>75</v>
       </c>
-      <c r="J17" s="11" t="s">
-        <v>53</v>
+      <c r="J17" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="K17" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="L17" s="24" t="s">
+      <c r="L17" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="M17" s="24" t="s">
+      <c r="M17" s="15" t="s">
         <v>32</v>
       </c>
       <c r="N17" s="7">
@@ -1365,26 +1400,26 @@
       <c r="O17" s="7">
         <v>12</v>
       </c>
-      <c r="P17" s="24" t="s">
+      <c r="P17" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="Q17" s="24"/>
+      <c r="Q17" s="15"/>
       <c r="R17" s="9" t="s">
         <v>12</v>
       </c>
       <c r="S17" s="9"/>
     </row>
     <row r="18" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J18" s="11" t="s">
+      <c r="J18" s="28" t="s">
         <v>61</v>
       </c>
       <c r="K18" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="L18" s="24" t="s">
+      <c r="L18" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="M18" s="24" t="s">
+      <c r="M18" s="15" t="s">
         <v>33</v>
       </c>
       <c r="N18" s="7">
@@ -1393,26 +1428,26 @@
       <c r="O18" s="7">
         <v>13</v>
       </c>
-      <c r="P18" s="24" t="s">
+      <c r="P18" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="Q18" s="24"/>
+      <c r="Q18" s="15"/>
       <c r="R18" s="9" t="s">
         <v>13</v>
       </c>
       <c r="S18" s="9"/>
     </row>
     <row r="19" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J19" s="11" t="s">
+      <c r="J19" s="28" t="s">
         <v>62</v>
       </c>
       <c r="K19" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="L19" s="24" t="s">
+      <c r="L19" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="M19" s="24" t="s">
+      <c r="M19" s="15" t="s">
         <v>34</v>
       </c>
       <c r="N19" s="7">
@@ -1421,10 +1456,10 @@
       <c r="O19" s="7">
         <v>14</v>
       </c>
-      <c r="P19" s="24" t="s">
+      <c r="P19" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="Q19" s="24" t="s">
+      <c r="Q19" s="15" t="s">
         <v>47</v>
       </c>
       <c r="R19" s="9" t="s">
@@ -1435,16 +1470,16 @@
       </c>
     </row>
     <row r="20" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J20" s="10" t="s">
+      <c r="J20" s="29" t="s">
         <v>63</v>
       </c>
       <c r="K20" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="L20" s="24" t="s">
+      <c r="L20" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="M20" s="24" t="s">
+      <c r="M20" s="15" t="s">
         <v>35</v>
       </c>
       <c r="N20" s="7">
@@ -1453,10 +1488,10 @@
       <c r="O20" s="7">
         <v>15</v>
       </c>
-      <c r="P20" s="24" t="s">
+      <c r="P20" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="Q20" s="24" t="s">
+      <c r="Q20" s="15" t="s">
         <v>48</v>
       </c>
       <c r="R20" s="9" t="s">
@@ -1467,19 +1502,19 @@
       </c>
     </row>
     <row r="21" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I21" s="15" t="s">
+      <c r="I21" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="J21" s="12" t="s">
+      <c r="J21" s="27" t="s">
         <v>56</v>
       </c>
       <c r="K21" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="L21" s="24" t="s">
+      <c r="L21" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="M21" s="24" t="s">
+      <c r="M21" s="15" t="s">
         <v>36</v>
       </c>
       <c r="N21" s="7">
@@ -1488,27 +1523,27 @@
       <c r="O21" s="7">
         <v>16</v>
       </c>
-      <c r="P21" s="24" t="s">
+      <c r="P21" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="Q21" s="24"/>
+      <c r="Q21" s="15"/>
       <c r="R21" s="9" t="s">
         <v>16</v>
       </c>
       <c r="S21" s="9"/>
     </row>
     <row r="22" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I22" s="15" t="s">
+      <c r="I22" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="J22" s="10" t="s">
+      <c r="J22" s="23" t="s">
         <v>54</v>
       </c>
       <c r="K22" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="L22" s="24"/>
-      <c r="M22" s="24" t="s">
+      <c r="L22" s="15"/>
+      <c r="M22" s="15" t="s">
         <v>37</v>
       </c>
       <c r="N22" s="7">
@@ -1517,16 +1552,16 @@
       <c r="O22" s="7">
         <v>17</v>
       </c>
-      <c r="P22" s="24" t="s">
+      <c r="P22" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="Q22" s="24" t="s">
+      <c r="Q22" s="15" t="s">
         <v>55</v>
       </c>
       <c r="R22" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="S22" s="10" t="s">
+      <c r="S22" s="23" t="s">
         <v>55</v>
       </c>
       <c r="T22" t="s">
@@ -1538,8 +1573,8 @@
       <c r="K23" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="L23" s="24"/>
-      <c r="M23" s="24" t="s">
+      <c r="L23" s="15"/>
+      <c r="M23" s="15" t="s">
         <v>38</v>
       </c>
       <c r="N23" s="7">
@@ -1548,10 +1583,10 @@
       <c r="O23" s="7">
         <v>18</v>
       </c>
-      <c r="P23" s="24" t="s">
+      <c r="P23" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="Q23" s="24"/>
+      <c r="Q23" s="15"/>
       <c r="R23" s="8" t="s">
         <v>18</v>
       </c>
@@ -1562,8 +1597,8 @@
       <c r="K24" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="L24" s="24"/>
-      <c r="M24" s="24" t="s">
+      <c r="L24" s="15"/>
+      <c r="M24" s="15" t="s">
         <v>2</v>
       </c>
       <c r="N24" s="7">
@@ -1572,10 +1607,10 @@
       <c r="O24" s="7">
         <v>19</v>
       </c>
-      <c r="P24" s="24" t="s">
+      <c r="P24" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="Q24" s="24"/>
+      <c r="Q24" s="15"/>
       <c r="R24" s="8" t="s">
         <v>19</v>
       </c>
@@ -1586,8 +1621,8 @@
       <c r="K25" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L25" s="24"/>
-      <c r="M25" s="24" t="s">
+      <c r="L25" s="15"/>
+      <c r="M25" s="15" t="s">
         <v>2</v>
       </c>
       <c r="N25" s="7">
@@ -1596,16 +1631,16 @@
       <c r="O25" s="7">
         <v>20</v>
       </c>
-      <c r="P25" s="24" t="s">
+      <c r="P25" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="Q25" s="24" t="s">
+      <c r="Q25" s="15" t="s">
         <v>57</v>
       </c>
       <c r="R25" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="S25" s="10" t="s">
+      <c r="S25" s="26" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se actualiza codigo fuente
</commit_message>
<xml_diff>
--- a/Pinout STM32.xlsx
+++ b/Pinout STM32.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RepositoriosGit\EstacionCalorPro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27A5718-BAB4-4FA2-99AA-EE0E3016ED78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3540F7A-9900-4224-BB4D-D44B875C6B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F50C8D62-0681-441D-8638-5078836FED94}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F50C8D62-0681-441D-8638-5078836FED94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="87">
   <si>
     <t>Pin</t>
   </si>
@@ -260,9 +260,6 @@
     <t>A3 (ADC1_IN3)</t>
   </si>
   <si>
-    <t>GPIO_EXTI4</t>
-  </si>
-  <si>
     <t>GPIO_EXTI6</t>
   </si>
   <si>
@@ -281,9 +278,6 @@
     <t>sensor teperatura analogico</t>
   </si>
   <si>
-    <t>Boton2</t>
-  </si>
-  <si>
     <t>GPIO_EXTI13</t>
   </si>
   <si>
@@ -291,6 +285,18 @@
   </si>
   <si>
     <t>zumbador</t>
+  </si>
+  <si>
+    <t>BOTON-Manual</t>
+  </si>
+  <si>
+    <t>BOTON-Memoria1</t>
+  </si>
+  <si>
+    <t>Boton-Memoria2</t>
+  </si>
+  <si>
+    <t>BOTON-Memoria3</t>
   </si>
 </sst>
 </file>
@@ -340,7 +346,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -368,12 +374,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -460,7 +460,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -479,17 +479,18 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -975,7 +976,7 @@
   <dimension ref="I2:T25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="T19" sqref="T19:T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -995,28 +996,28 @@
   <sheetData>
     <row r="2" spans="9:20" x14ac:dyDescent="0.25">
       <c r="J2" s="2"/>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
       <c r="S2" s="2"/>
     </row>
     <row r="3" spans="9:20" x14ac:dyDescent="0.25">
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="24" t="s">
+      <c r="M3" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
@@ -1026,46 +1027,46 @@
       <c r="K4" s="2"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="23" t="s">
+      <c r="N4" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="O4" s="23"/>
+      <c r="O4" s="24"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
     </row>
     <row r="5" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J5" s="28" t="s">
+      <c r="J5" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="K5" s="29"/>
-      <c r="L5" s="26" t="s">
+      <c r="K5" s="30"/>
+      <c r="L5" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="M5" s="27"/>
+      <c r="M5" s="28"/>
       <c r="N5" s="5" t="s">
         <v>0</v>
       </c>
       <c r="O5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="P5" s="26" t="s">
+      <c r="P5" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="Q5" s="27"/>
-      <c r="R5" s="28" t="s">
+      <c r="Q5" s="28"/>
+      <c r="R5" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="S5" s="29"/>
+      <c r="S5" s="30"/>
     </row>
     <row r="6" spans="9:20" x14ac:dyDescent="0.25">
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15" t="s">
+      <c r="L6" s="14"/>
+      <c r="M6" s="14" t="s">
         <v>21</v>
       </c>
       <c r="N6" s="5">
@@ -1074,27 +1075,28 @@
       <c r="O6" s="5">
         <v>1</v>
       </c>
-      <c r="P6" s="15" t="s">
+      <c r="P6" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="Q6" s="15"/>
+      <c r="Q6" s="14"/>
       <c r="R6" s="4" t="s">
         <v>1</v>
       </c>
       <c r="S6" s="4"/>
+      <c r="T6" s="22"/>
     </row>
     <row r="7" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I7" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="J7" s="17" t="s">
-        <v>52</v>
+      <c r="I7" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>84</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15" t="s">
+      <c r="L7" s="14"/>
+      <c r="M7" s="14" t="s">
         <v>22</v>
       </c>
       <c r="N7" s="7">
@@ -1103,22 +1105,23 @@
       <c r="O7" s="7">
         <v>2</v>
       </c>
-      <c r="P7" s="15" t="s">
+      <c r="P7" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="Q7" s="15"/>
+      <c r="Q7" s="14"/>
       <c r="R7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="S7" s="4"/>
+      <c r="T7" s="22"/>
     </row>
     <row r="8" spans="9:20" x14ac:dyDescent="0.25">
       <c r="J8" s="4"/>
       <c r="K8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15" t="s">
+      <c r="L8" s="14"/>
+      <c r="M8" s="14" t="s">
         <v>23</v>
       </c>
       <c r="N8" s="7">
@@ -1127,22 +1130,23 @@
       <c r="O8" s="7">
         <v>3</v>
       </c>
-      <c r="P8" s="15" t="s">
+      <c r="P8" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="Q8" s="15"/>
+      <c r="Q8" s="14"/>
       <c r="R8" s="4" t="s">
         <v>3</v>
       </c>
       <c r="S8" s="4"/>
+      <c r="T8" s="22"/>
     </row>
     <row r="9" spans="9:20" x14ac:dyDescent="0.25">
       <c r="J9" s="4"/>
       <c r="K9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15" t="s">
+      <c r="L9" s="14"/>
+      <c r="M9" s="14" t="s">
         <v>24</v>
       </c>
       <c r="N9" s="7">
@@ -1151,23 +1155,24 @@
       <c r="O9" s="7">
         <v>4</v>
       </c>
-      <c r="P9" s="15" t="s">
+      <c r="P9" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="Q9" s="15"/>
+      <c r="Q9" s="14"/>
       <c r="R9" s="8" t="s">
         <v>4</v>
       </c>
+      <c r="S9" s="4"/>
     </row>
     <row r="10" spans="9:20" x14ac:dyDescent="0.25">
       <c r="J10" s="4"/>
       <c r="K10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="L10" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="M10" s="15" t="s">
+      <c r="M10" s="14" t="s">
         <v>25</v>
       </c>
       <c r="N10" s="7">
@@ -1176,20 +1181,20 @@
       <c r="O10" s="7">
         <v>5</v>
       </c>
-      <c r="P10" s="15" t="s">
+      <c r="P10" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="Q10" s="15" t="s">
+      <c r="Q10" s="14" t="s">
         <v>58</v>
       </c>
       <c r="R10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="S10" s="19" t="s">
+      <c r="S10" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="T10" t="s">
-        <v>77</v>
+      <c r="T10" s="22" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="9:20" x14ac:dyDescent="0.25">
@@ -1197,10 +1202,10 @@
       <c r="K11" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="L11" s="15" t="s">
+      <c r="L11" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="M11" s="15" t="s">
+      <c r="M11" s="14" t="s">
         <v>26</v>
       </c>
       <c r="N11" s="7">
@@ -1209,10 +1214,10 @@
       <c r="O11" s="7">
         <v>6</v>
       </c>
-      <c r="P11" s="15" t="s">
+      <c r="P11" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="Q11" s="15" t="s">
+      <c r="Q11" s="14" t="s">
         <v>46</v>
       </c>
       <c r="R11" s="8" t="s">
@@ -1221,16 +1226,17 @@
       <c r="S11" s="10" t="s">
         <v>46</v>
       </c>
+      <c r="T11" s="22"/>
     </row>
     <row r="12" spans="9:20" x14ac:dyDescent="0.25">
       <c r="J12" s="11"/>
       <c r="K12" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="L12" s="15" t="s">
+      <c r="L12" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="15" t="s">
+      <c r="M12" s="14" t="s">
         <v>27</v>
       </c>
       <c r="N12" s="7">
@@ -1239,10 +1245,10 @@
       <c r="O12" s="7">
         <v>7</v>
       </c>
-      <c r="P12" s="15" t="s">
+      <c r="P12" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="Q12" s="15" t="s">
+      <c r="Q12" s="14" t="s">
         <v>45</v>
       </c>
       <c r="R12" s="8" t="s">
@@ -1251,18 +1257,20 @@
       <c r="S12" s="10" t="s">
         <v>45</v>
       </c>
+      <c r="T12" s="22"/>
     </row>
     <row r="13" spans="9:20" x14ac:dyDescent="0.25">
+      <c r="I13" s="22"/>
       <c r="J13" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K13" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="L13" s="15" t="s">
+      <c r="L13" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="M13" s="15" t="s">
+      <c r="M13" s="14" t="s">
         <v>28</v>
       </c>
       <c r="N13" s="7">
@@ -1271,10 +1279,10 @@
       <c r="O13" s="7">
         <v>8</v>
       </c>
-      <c r="P13" s="15" t="s">
+      <c r="P13" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="Q13" s="15" t="s">
+      <c r="Q13" s="14" t="s">
         <v>49</v>
       </c>
       <c r="R13" s="8" t="s">
@@ -1283,18 +1291,20 @@
       <c r="S13" s="10" t="s">
         <v>49</v>
       </c>
+      <c r="T13" s="22"/>
     </row>
     <row r="14" spans="9:20" x14ac:dyDescent="0.25">
+      <c r="I14" s="22"/>
       <c r="J14" s="11" t="s">
         <v>59</v>
       </c>
       <c r="K14" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="L14" s="15" t="s">
+      <c r="L14" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="M14" s="15" t="s">
+      <c r="M14" s="14" t="s">
         <v>29</v>
       </c>
       <c r="N14" s="7">
@@ -1303,33 +1313,30 @@
       <c r="O14" s="7">
         <v>9</v>
       </c>
-      <c r="P14" s="15" t="s">
+      <c r="P14" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="Q14" s="15" t="s">
+      <c r="Q14" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="R14" s="12" t="s">
+      <c r="R14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="S14" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="T14" s="13" t="s">
-        <v>74</v>
-      </c>
+      <c r="S14" s="4"/>
+      <c r="T14" s="12"/>
     </row>
     <row r="15" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J15" s="14" t="s">
-        <v>80</v>
+      <c r="I15" s="22"/>
+      <c r="J15" s="13" t="s">
+        <v>79</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="L15" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="L15" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="M15" s="15" t="s">
+      <c r="M15" s="14" t="s">
         <v>30</v>
       </c>
       <c r="N15" s="7">
@@ -1338,10 +1345,10 @@
       <c r="O15" s="7">
         <v>10</v>
       </c>
-      <c r="P15" s="15" t="s">
+      <c r="P15" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="Q15" s="15" t="s">
+      <c r="Q15" s="14" t="s">
         <v>51</v>
       </c>
       <c r="R15" s="8" t="s">
@@ -1350,18 +1357,20 @@
       <c r="S15" s="10" t="s">
         <v>51</v>
       </c>
+      <c r="T15" s="22"/>
     </row>
     <row r="16" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J16" s="21" t="s">
+      <c r="I16" s="22"/>
+      <c r="J16" s="20" t="s">
         <v>60</v>
       </c>
       <c r="K16" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="L16" s="15" t="s">
+      <c r="L16" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="M16" s="15" t="s">
+      <c r="M16" s="14" t="s">
         <v>31</v>
       </c>
       <c r="N16" s="7">
@@ -1370,10 +1379,10 @@
       <c r="O16" s="7">
         <v>11</v>
       </c>
-      <c r="P16" s="15" t="s">
+      <c r="P16" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="Q16" s="15" t="s">
+      <c r="Q16" s="14" t="s">
         <v>50</v>
       </c>
       <c r="R16" s="9" t="s">
@@ -1382,21 +1391,22 @@
       <c r="S16" s="11" t="s">
         <v>50</v>
       </c>
+      <c r="T16" s="22"/>
     </row>
     <row r="17" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I17" t="s">
-        <v>75</v>
-      </c>
-      <c r="J17" s="18" t="s">
-        <v>81</v>
+      <c r="I17" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="J17" s="17" t="s">
+        <v>85</v>
       </c>
       <c r="K17" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="L17" s="15" t="s">
+      <c r="L17" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="M17" s="15" t="s">
+      <c r="M17" s="14" t="s">
         <v>32</v>
       </c>
       <c r="N17" s="7">
@@ -1405,26 +1415,27 @@
       <c r="O17" s="7">
         <v>12</v>
       </c>
-      <c r="P17" s="15" t="s">
+      <c r="P17" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="Q17" s="15"/>
+      <c r="Q17" s="14"/>
       <c r="R17" s="9" t="s">
         <v>12</v>
       </c>
       <c r="S17" s="9"/>
     </row>
     <row r="18" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J18" s="21" t="s">
+      <c r="I18" s="22"/>
+      <c r="J18" s="20" t="s">
         <v>61</v>
       </c>
       <c r="K18" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="L18" s="15" t="s">
+      <c r="L18" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="M18" s="15" t="s">
+      <c r="M18" s="14" t="s">
         <v>33</v>
       </c>
       <c r="N18" s="7">
@@ -1433,26 +1444,27 @@
       <c r="O18" s="7">
         <v>13</v>
       </c>
-      <c r="P18" s="15" t="s">
+      <c r="P18" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="Q18" s="15"/>
+      <c r="Q18" s="14"/>
       <c r="R18" s="9" t="s">
         <v>13</v>
       </c>
       <c r="S18" s="9"/>
     </row>
     <row r="19" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J19" s="21" t="s">
+      <c r="I19" s="22"/>
+      <c r="J19" s="20" t="s">
         <v>62</v>
       </c>
       <c r="K19" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="L19" s="15" t="s">
+      <c r="L19" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="M19" s="15" t="s">
+      <c r="M19" s="14" t="s">
         <v>34</v>
       </c>
       <c r="N19" s="7">
@@ -1461,10 +1473,10 @@
       <c r="O19" s="7">
         <v>14</v>
       </c>
-      <c r="P19" s="15" t="s">
+      <c r="P19" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="Q19" s="15" t="s">
+      <c r="Q19" s="14" t="s">
         <v>47</v>
       </c>
       <c r="R19" s="9" t="s">
@@ -1473,18 +1485,20 @@
       <c r="S19" s="11" t="s">
         <v>47</v>
       </c>
+      <c r="T19" s="22"/>
     </row>
     <row r="20" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="J20" s="22" t="s">
+      <c r="I20" s="22"/>
+      <c r="J20" s="21" t="s">
         <v>63</v>
       </c>
       <c r="K20" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="L20" s="15" t="s">
+      <c r="L20" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="M20" s="15" t="s">
+      <c r="M20" s="14" t="s">
         <v>35</v>
       </c>
       <c r="N20" s="7">
@@ -1493,10 +1507,10 @@
       <c r="O20" s="7">
         <v>15</v>
       </c>
-      <c r="P20" s="15" t="s">
+      <c r="P20" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="Q20" s="15" t="s">
+      <c r="Q20" s="14" t="s">
         <v>48</v>
       </c>
       <c r="R20" s="9" t="s">
@@ -1505,21 +1519,22 @@
       <c r="S20" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="T20" s="22"/>
     </row>
     <row r="21" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I21" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="J21" s="20" t="s">
+      <c r="I21" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="J21" s="19" t="s">
         <v>56</v>
       </c>
       <c r="K21" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="L21" s="15" t="s">
+      <c r="L21" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="M21" s="15" t="s">
+      <c r="M21" s="14" t="s">
         <v>36</v>
       </c>
       <c r="N21" s="7">
@@ -1528,27 +1543,27 @@
       <c r="O21" s="7">
         <v>16</v>
       </c>
-      <c r="P21" s="15" t="s">
+      <c r="P21" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="Q21" s="15"/>
+      <c r="Q21" s="14"/>
       <c r="R21" s="9" t="s">
         <v>16</v>
       </c>
       <c r="S21" s="9"/>
     </row>
     <row r="22" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I22" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="J22" s="16" t="s">
-        <v>54</v>
+      <c r="I22" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="J22" s="15" t="s">
+        <v>86</v>
       </c>
       <c r="K22" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15" t="s">
+      <c r="L22" s="14"/>
+      <c r="M22" s="14" t="s">
         <v>37</v>
       </c>
       <c r="N22" s="7">
@@ -1557,29 +1572,30 @@
       <c r="O22" s="7">
         <v>17</v>
       </c>
-      <c r="P22" s="15" t="s">
+      <c r="P22" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="Q22" s="15" t="s">
+      <c r="Q22" s="14" t="s">
         <v>55</v>
       </c>
       <c r="R22" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="S22" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="T22" t="s">
-        <v>79</v>
+      <c r="S22" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="T22" s="22" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="9:20" x14ac:dyDescent="0.25">
+      <c r="I23" s="22"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15" t="s">
+      <c r="L23" s="14"/>
+      <c r="M23" s="14" t="s">
         <v>38</v>
       </c>
       <c r="N23" s="7">
@@ -1588,22 +1604,23 @@
       <c r="O23" s="7">
         <v>18</v>
       </c>
-      <c r="P23" s="15" t="s">
+      <c r="P23" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="Q23" s="15"/>
+      <c r="Q23" s="14"/>
       <c r="R23" s="8" t="s">
         <v>18</v>
       </c>
       <c r="S23" s="8"/>
     </row>
     <row r="24" spans="9:20" x14ac:dyDescent="0.25">
+      <c r="I24" s="22"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15" t="s">
+      <c r="L24" s="14"/>
+      <c r="M24" s="14" t="s">
         <v>2</v>
       </c>
       <c r="N24" s="7">
@@ -1612,22 +1629,23 @@
       <c r="O24" s="7">
         <v>19</v>
       </c>
-      <c r="P24" s="15" t="s">
+      <c r="P24" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q24" s="15"/>
+      <c r="Q24" s="14"/>
       <c r="R24" s="8" t="s">
         <v>19</v>
       </c>
       <c r="S24" s="8"/>
     </row>
     <row r="25" spans="9:20" x14ac:dyDescent="0.25">
+      <c r="I25" s="22"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15" t="s">
+      <c r="L25" s="14"/>
+      <c r="M25" s="14" t="s">
         <v>2</v>
       </c>
       <c r="N25" s="7">
@@ -1636,18 +1654,19 @@
       <c r="O25" s="7">
         <v>20</v>
       </c>
-      <c r="P25" s="15" t="s">
+      <c r="P25" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="Q25" s="15" t="s">
+      <c r="Q25" s="14" t="s">
         <v>57</v>
       </c>
       <c r="R25" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="S25" s="19" t="s">
+      <c r="S25" s="18" t="s">
         <v>57</v>
       </c>
+      <c r="T25" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>